<commit_message>
- added screenshot method
- added basecase method that will handle all of the test suite set up
before running each test case.

- implemented extent report libraries for better detail reporting
</commit_message>
<xml_diff>
--- a/ HybridFramwork /TestData/ProjectData.xlsx
+++ b/ HybridFramwork /TestData/ProjectData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagmandeepdhaliwal/eclipse-workspace/ HybridFramwork /TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagmandeepdhaliwal/git/Framework/ HybridFramwork /TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143FE705-583E-2B4B-BB6A-6F958BBD7D04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F326B87-0FD8-B042-8C4A-E61FA2D67EF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{D97A505A-FF7C-624F-8CA6-A4A6142DE3F4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16020" xr2:uid="{D97A505A-FF7C-624F-8CA6-A4A6142DE3F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F6106B-C841-7841-805B-52901F196584}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -417,7 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A83197-74AD-8341-8508-1F273C6DF0AB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>